<commit_message>
rest assured testng.xml added.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/userData.xlsx
+++ b/src/test/resources/testData/userData.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -48,19 +48,29 @@
     <t>active</t>
   </si>
   <si>
-    <t>alexde@test.on</t>
-  </si>
-  <si>
-    <t>canbartu@test.on</t>
-  </si>
-  <si>
-    <t>senturks@test.on</t>
+    <t>alexde@test.f</t>
+  </si>
+  <si>
+    <t>canbartu@test.f</t>
+  </si>
+  <si>
+    <t>senturks@test.f</t>
+  </si>
+  <si>
+    <t>5841117</t>
+  </si>
+  <si>
+    <t>5841118</t>
+  </si>
+  <si>
+    <t>5841119</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,19 +407,19 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="14.0"/>
+    <col min="2" max="2" style="1" width="9.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="18.5703125"/>
+    <col min="4" max="4" customWidth="true" style="1" width="9.140625"/>
+    <col min="5" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -439,6 +449,9 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -453,6 +466,9 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -466,6 +482,9 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F4" t="s" s="1">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -477,12 +496,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddHeader>
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddFooter>
-    <evenHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenHeader>
-    <evenFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenFooter>
-    <firstHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstHeader>
-    <firstFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstFooter>
+    <oddHeader><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></oddHeader>
+    <oddFooter><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></oddFooter>
+    <evenHeader><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></evenHeader>
+    <evenFooter><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></evenFooter>
+    <firstHeader><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></firstHeader>
+    <firstFooter><![CDATA[&L&"Arial,Regular"&09&B&U&K000000TASNİF DIŞI&K0000FF &B&K663987/ &I&K663987UNCLASSIFIED]]></firstFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -494,7 +513,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66403C9F-D114-41CD-A286-35FB16205129}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FEDFD6D-5439-4461-931C-DB076E4759DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>